<commit_message>
Excel Utility added. Listners interface added. POM updated for Extent report dpendencies. testng xml updated for listners.
</commit_message>
<xml_diff>
--- a/src/main/resources/Form_Data.xlsx
+++ b/src/main/resources/Form_Data.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17430" windowHeight="4965"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17805" windowHeight="4470"/>
   </bookViews>
   <sheets>
-    <sheet name="New_Org_data" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="eOasis_Credentials" sheetId="2" r:id="rId1"/>
+    <sheet name="TC42404" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:Q13"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Address_Line1</t>
   </si>
@@ -50,13 +50,25 @@
   </si>
   <si>
     <t>Area_code</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>vthorat</t>
+  </si>
+  <si>
+    <t>M@G580746</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,16 +84,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -89,21 +115,128 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -403,10 +536,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,61 +589,49 @@
     <col min="6" max="6" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="5">
         <v>471</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="6" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Wait added in common action class. Pdf reader chagnes. Updated excel sheet[test data]
</commit_message>
<xml_diff>
--- a/src/main/resources/Form_Data.xlsx
+++ b/src/main/resources/Form_Data.xlsx
@@ -4,20 +4,27 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17805" windowHeight="4470"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15090" windowHeight="3885" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
-    <sheet name="eOasis_Credentials" sheetId="2" r:id="rId1"/>
+    <sheet name="TC42665" sheetId="2" r:id="rId1"/>
     <sheet name="TC42404" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="TC42239" sheetId="3" r:id="rId3"/>
+    <sheet name="TC42242" sheetId="4" r:id="rId4"/>
+    <sheet name="TC42238" sheetId="5" r:id="rId5"/>
+    <sheet name="TC42245" sheetId="6" r:id="rId6"/>
+    <sheet name="TC_Indication" sheetId="7" r:id="rId7"/>
+    <sheet name="TC42530" sheetId="8" r:id="rId8"/>
+    <sheet name="TC42536" sheetId="9" r:id="rId9"/>
+    <sheet name="Quick_Add" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:Q13"/>
+  <oleSize ref="A1:O11"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="15">
   <si>
     <t>Address_Line1</t>
   </si>
@@ -536,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,7 +555,7 @@
     <col min="2" max="2" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
@@ -556,7 +563,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>13</v>
       </c>
@@ -570,6 +577,44 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -637,12 +682,264 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Page Object class name changes.
</commit_message>
<xml_diff>
--- a/src/main/resources/Form_Data.xlsx
+++ b/src/main/resources/Form_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15090" windowHeight="3885" firstSheet="3" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="16305" windowHeight="3885" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TC42665" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Quick_Add" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:O11"/>
+  <oleSize ref="A1:S19"/>
 </workbook>
 </file>
 
@@ -584,7 +584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
@@ -723,7 +723,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,7 +798,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Create CLaim TC, PDF autoIt script updated[Save PDf path updated] Claims PO & DTO created
</commit_message>
<xml_diff>
--- a/src/main/resources/Form_Data.xlsx
+++ b/src/main/resources/Form_Data.xlsx
@@ -4,29 +4,30 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2448" windowWidth="23136" windowHeight="11076" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="20580" windowHeight="11070" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TC42400" sheetId="12" r:id="rId1"/>
     <sheet name="TC43666" sheetId="14" r:id="rId2"/>
-    <sheet name="TC42665" sheetId="2" r:id="rId3"/>
-    <sheet name="HomePageData" sheetId="11" r:id="rId4"/>
-    <sheet name="TC42404" sheetId="1" r:id="rId5"/>
-    <sheet name="TC42239" sheetId="3" r:id="rId6"/>
-    <sheet name="TC42242" sheetId="4" r:id="rId7"/>
-    <sheet name="TC42238" sheetId="5" r:id="rId8"/>
-    <sheet name="TC42245" sheetId="6" r:id="rId9"/>
-    <sheet name="TC_Indication" sheetId="13" r:id="rId10"/>
-    <sheet name="TC42530" sheetId="8" r:id="rId11"/>
-    <sheet name="TC42536" sheetId="9" r:id="rId12"/>
-    <sheet name="Quick_Add" sheetId="10" r:id="rId13"/>
+    <sheet name="TC42405" sheetId="15" r:id="rId3"/>
+    <sheet name="TC42665" sheetId="2" r:id="rId4"/>
+    <sheet name="HomePageData" sheetId="11" r:id="rId5"/>
+    <sheet name="TC42404" sheetId="1" r:id="rId6"/>
+    <sheet name="TC42239" sheetId="3" r:id="rId7"/>
+    <sheet name="TC42242" sheetId="4" r:id="rId8"/>
+    <sheet name="TC42238" sheetId="5" r:id="rId9"/>
+    <sheet name="TC42245" sheetId="6" r:id="rId10"/>
+    <sheet name="TC_Indication" sheetId="13" r:id="rId11"/>
+    <sheet name="TC42530" sheetId="8" r:id="rId12"/>
+    <sheet name="TC42536" sheetId="9" r:id="rId13"/>
+    <sheet name="Quick_Add" sheetId="10" r:id="rId14"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="132">
   <si>
     <t>Address_Line1</t>
   </si>
@@ -981,13 +982,13 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
@@ -995,7 +996,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>13</v>
       </c>
@@ -1013,309 +1014,32 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD7"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.6640625" customWidth="1"/>
-    <col min="15" max="15" width="11.109375" customWidth="1"/>
-    <col min="16" max="16" width="15.6640625" customWidth="1"/>
-    <col min="17" max="17" width="11.88671875" customWidth="1"/>
-    <col min="18" max="18" width="15.5546875" customWidth="1"/>
-    <col min="19" max="19" width="11.44140625" customWidth="1"/>
-    <col min="20" max="20" width="28.109375" customWidth="1"/>
-    <col min="21" max="21" width="10.6640625" customWidth="1"/>
-    <col min="22" max="22" width="11.88671875" customWidth="1"/>
-    <col min="23" max="23" width="19" customWidth="1"/>
-    <col min="24" max="24" width="11.44140625" customWidth="1"/>
-    <col min="25" max="25" width="12.77734375" customWidth="1"/>
-    <col min="26" max="26" width="12.21875" customWidth="1"/>
-    <col min="27" max="27" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="20" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="J1" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="K1" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="L1" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="M1" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="N1" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="O1" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="P1" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q1" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="R1" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="S1" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="T1" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="U1" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="V1" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="W1" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="X1" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y1" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="Z1" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA1" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="AB1" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC1" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="AD1" s="22" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:30" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N2" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="O2" t="s">
-        <v>49</v>
-      </c>
-      <c r="P2" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q2" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="R2" t="s">
-        <v>51</v>
-      </c>
-      <c r="S2" t="s">
-        <v>60</v>
-      </c>
-      <c r="T2" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="U2" t="s">
-        <v>59</v>
-      </c>
-      <c r="V2" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="W2" t="s">
-        <v>44</v>
-      </c>
-      <c r="X2" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>65</v>
-      </c>
-      <c r="Z2" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="G3" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K3" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="M3" t="s">
-        <v>40</v>
-      </c>
-      <c r="N3" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>78</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="J4" t="s">
-        <v>38</v>
-      </c>
-      <c r="K4" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="L4" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="M4" t="s">
-        <v>41</v>
-      </c>
-      <c r="N4" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="M5" t="s">
-        <v>42</v>
-      </c>
-      <c r="N5" s="23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="M6" t="s">
-        <v>43</v>
-      </c>
-      <c r="N6" s="23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="M7" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1328,35 +1052,315 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:AD7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" customWidth="1"/>
+    <col min="18" max="18" width="15.5703125" customWidth="1"/>
+    <col min="19" max="19" width="11.42578125" customWidth="1"/>
+    <col min="20" max="20" width="28.140625" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" customWidth="1"/>
+    <col min="22" max="22" width="11.85546875" customWidth="1"/>
+    <col min="23" max="23" width="19" customWidth="1"/>
+    <col min="24" max="24" width="11.42578125" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" customWidth="1"/>
+    <col min="26" max="26" width="12.28515625" customWidth="1"/>
+    <col min="27" max="27" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:30" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="C1" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="P1" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="R1" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="S1" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="T1" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="U1" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="V1" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="W1" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="X1" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y1" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z1" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA1" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB1" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC1" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD1" s="22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" ht="43.9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="12" t="s">
         <v>14</v>
       </c>
+      <c r="C2" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" t="s">
+        <v>49</v>
+      </c>
+      <c r="P2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q2" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="R2" t="s">
+        <v>51</v>
+      </c>
+      <c r="S2" t="s">
+        <v>60</v>
+      </c>
+      <c r="T2" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="U2" t="s">
+        <v>59</v>
+      </c>
+      <c r="V2" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="W2" t="s">
+        <v>44</v>
+      </c>
+      <c r="X2" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z2" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="G3" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="J4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" t="s">
+        <v>41</v>
+      </c>
+      <c r="N4" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="M5" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="M6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="M7" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1366,35 +1370,32 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1407,13 +1408,13 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
@@ -1421,7 +1422,45 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>13</v>
       </c>
@@ -1442,23 +1481,23 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -1553,29 +1592,74 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
-    <col min="4" max="4" width="38.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.21875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1738,7 +1822,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1746,12 +1830,12 @@
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1788,29 +1872,29 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="7" width="12.44140625" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="13" max="13" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1851,7 +1935,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="58.15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>13</v>
       </c>
@@ -1901,21 +1985,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
@@ -1923,7 +2007,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>13</v>
       </c>
@@ -1939,7 +2023,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
@@ -1947,15 +2031,15 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2042,72 +2126,41 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C1" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>14</v>
       </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>14</v>
+      <c r="C2" s="11" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Smoke test cases udpate java class for execution ANd code to write policy / Claim no in excel
</commit_message>
<xml_diff>
--- a/src/main/resources/Form_Data.xlsx
+++ b/src/main/resources/Form_Data.xlsx
@@ -1,37 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="17" firstSheet="13" windowHeight="11070" windowWidth="20580" xWindow="0" yWindow="2445"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="20580" windowHeight="11070" firstSheet="13" activeTab="16"/>
   </bookViews>
   <sheets>
-    <sheet name="TC42400" r:id="rId1" sheetId="12"/>
-    <sheet name="TC43666" r:id="rId2" sheetId="14"/>
-    <sheet name="TC42243" r:id="rId3" sheetId="16"/>
-    <sheet name="TC42405" r:id="rId4" sheetId="15"/>
-    <sheet name="TC42665" r:id="rId5" sheetId="2"/>
-    <sheet name="HomePageData" r:id="rId6" sheetId="11"/>
-    <sheet name="TC42404" r:id="rId7" sheetId="1"/>
-    <sheet name="TC42239" r:id="rId8" sheetId="3"/>
-    <sheet name="TC42242" r:id="rId9" sheetId="4"/>
-    <sheet name="TC42238" r:id="rId10" sheetId="5"/>
-    <sheet name="TC42245" r:id="rId11" sheetId="6"/>
-    <sheet name="TC_Indication" r:id="rId12" sheetId="13"/>
-    <sheet name="TC42530" r:id="rId13" sheetId="8"/>
-    <sheet name="TC42536" r:id="rId14" sheetId="9"/>
-    <sheet name="Quick_Add" r:id="rId15" sheetId="10"/>
-    <sheet name="TC42240" r:id="rId16" sheetId="17"/>
-    <sheet name="TC42247" r:id="rId17" sheetId="18"/>
-    <sheet name="TC42250" r:id="rId18" sheetId="19"/>
+    <sheet name="TC42400" sheetId="12" r:id="rId1"/>
+    <sheet name="TC43666" sheetId="14" r:id="rId2"/>
+    <sheet name="TC42243" sheetId="16" r:id="rId3"/>
+    <sheet name="TC42405" sheetId="15" r:id="rId4"/>
+    <sheet name="TC42665" sheetId="2" r:id="rId5"/>
+    <sheet name="TC42399" sheetId="20" r:id="rId6"/>
+    <sheet name="HomePageData" sheetId="11" r:id="rId7"/>
+    <sheet name="TC42404" sheetId="1" r:id="rId8"/>
+    <sheet name="TC42239" sheetId="3" r:id="rId9"/>
+    <sheet name="TC42242" sheetId="4" r:id="rId10"/>
+    <sheet name="TC42238" sheetId="5" r:id="rId11"/>
+    <sheet name="TC42245" sheetId="6" r:id="rId12"/>
+    <sheet name="TC_Indication" sheetId="13" r:id="rId13"/>
+    <sheet name="TC42530" sheetId="8" r:id="rId14"/>
+    <sheet name="TC42536" sheetId="9" r:id="rId15"/>
+    <sheet name="Quick_Add" sheetId="10" r:id="rId16"/>
+    <sheet name="TC42240" sheetId="17" r:id="rId17"/>
+    <sheet name="TC42247" sheetId="18" r:id="rId18"/>
+    <sheet name="TC42250" sheetId="19" r:id="rId19"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="211">
   <si>
     <t>Address_Line1</t>
   </si>
@@ -621,32 +622,55 @@
     <t>09100232</t>
   </si>
   <si>
-    <t>3500052</t>
-  </si>
-  <si>
     <t>Number</t>
   </si>
   <si>
     <t>Amount</t>
   </si>
   <si>
-    <t>19862</t>
-  </si>
-  <si>
-    <t>19865</t>
-  </si>
-  <si>
-    <t>19866</t>
-  </si>
-  <si>
     <t>$0.00</t>
+  </si>
+  <si>
+    <t>09100197</t>
+  </si>
+  <si>
+    <t>TC42399</t>
+  </si>
+  <si>
+    <t>coverageFromCoverageTabGrid</t>
+  </si>
+  <si>
+    <t>manuscriptForm</t>
+  </si>
+  <si>
+    <t>viewModeOfficial</t>
+  </si>
+  <si>
+    <t>viewModeWIP</t>
+  </si>
+  <si>
+    <t>vbhalsing</t>
+  </si>
+  <si>
+    <t>M@G824829</t>
+  </si>
+  <si>
+    <t>HPL CHG 08</t>
+  </si>
+  <si>
+    <t>3500002A</t>
+  </si>
+  <si>
+    <t>WIP</t>
+  </si>
+  <si>
+    <t>HFL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -848,104 +872,119 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
+  <cellXfs count="50">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="3" fillId="0" fontId="0" numFmtId="14" quotePrefix="1" xfId="0">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="8" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyBorder="1" applyFont="1" borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="7" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyBorder="1" borderId="7" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="7" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="7" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="9" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="9" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="10" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="7" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="7" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="7" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyBorder="1" borderId="9" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="7" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="11" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="10" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -962,10 +1001,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1000,7 +1039,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1035,7 +1074,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1123,7 +1162,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -1132,13 +1171,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1148,7 +1187,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1157,7 +1196,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1166,7 +1205,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1176,12 +1215,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1212,7 +1251,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1231,7 +1270,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1243,8 +1282,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
@@ -1252,16 +1291,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="28" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="15.75" r="1" spans="1:7" thickBot="1">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
@@ -1284,7 +1323,7 @@
         <v>179</v>
       </c>
     </row>
-    <row ht="15.75" r="2" spans="1:7" thickBot="1">
+    <row r="2" spans="1:7" ht="15.75" thickBot="1">
       <c r="A2" s="11" t="s">
         <v>13</v>
       </c>
@@ -1307,36 +1346,146 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="23.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="15.75" r="1" spans="1:11" thickBot="1">
+    <row r="1" spans="1:10" s="1" customFormat="1">
+      <c r="A1" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="H3" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="H4" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="28" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" thickBot="1">
       <c r="A1" s="28" t="s">
         <v>11</v>
       </c>
@@ -1371,7 +1520,7 @@
         <v>180</v>
       </c>
     </row>
-    <row ht="15.75" r="2" spans="1:11" thickBot="1">
+    <row r="2" spans="1:11" ht="15.75" thickBot="1">
       <c r="A2" s="30" t="s">
         <v>13</v>
       </c>
@@ -1406,7 +1555,7 @@
         <v>143</v>
       </c>
     </row>
-    <row ht="15.75" r="3" spans="1:11" thickBot="1">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1">
       <c r="A3" s="30"/>
       <c r="B3" s="30"/>
       <c r="C3" s="30"/>
@@ -1421,7 +1570,7 @@
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
     </row>
-    <row ht="15.75" r="4" spans="1:11" thickBot="1">
+    <row r="4" spans="1:11" ht="15.75" thickBot="1">
       <c r="A4" s="30"/>
       <c r="B4" s="30"/>
       <c r="C4" s="30"/>
@@ -1438,28 +1587,28 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C2"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="15.75" r="1" spans="1:3" thickBot="1">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
@@ -1470,7 +1619,7 @@
         <v>148</v>
       </c>
     </row>
-    <row ht="15.75" r="2" spans="1:3" thickBot="1">
+    <row r="2" spans="1:3" ht="15.75" thickBot="1">
       <c r="A2" s="11" t="s">
         <v>13</v>
       </c>
@@ -1483,15 +1632,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE7"/>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AD7"/>
   <sheetViews>
     <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="W2" sqref="W2"/>
@@ -1499,38 +1648,38 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="28.140625" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="11.85546875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="11.42578125" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="28.140625" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="11.85546875" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="19" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="11.42578125" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="15.75" r="1" spans="1:30" thickBot="1">
+    <row r="1" spans="1:30" ht="15.75" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
@@ -1622,7 +1771,7 @@
         <v>81</v>
       </c>
     </row>
-    <row ht="45.75" r="2" spans="1:30" thickBot="1">
+    <row r="2" spans="1:30" ht="45.75" thickBot="1">
       <c r="A2" s="11" t="s">
         <v>13</v>
       </c>
@@ -1798,15 +1947,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -1814,8 +1963,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1835,13 +1984,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
@@ -1849,12 +1998,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="15.75" r="1" spans="1:3" thickBot="1">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
@@ -1865,7 +2014,7 @@
         <v>148</v>
       </c>
     </row>
-    <row ht="15.75" r="2" spans="1:3" thickBot="1">
+    <row r="2" spans="1:3" ht="15.75" thickBot="1">
       <c r="A2" s="11" t="s">
         <v>13</v>
       </c>
@@ -1878,15 +2027,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
@@ -1894,11 +2043,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="15.75" r="1" spans="1:2" thickBot="1">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
@@ -1906,7 +2055,7 @@
         <v>12</v>
       </c>
     </row>
-    <row ht="15.75" r="2" spans="1:2" thickBot="1">
+    <row r="2" spans="1:2" ht="15.75" thickBot="1">
       <c r="A2" s="11" t="s">
         <v>13</v>
       </c>
@@ -1916,32 +2065,32 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="31" spans="1:7">
+    <row r="1" spans="1:7" s="31" customFormat="1">
       <c r="A1" s="32" t="s">
         <v>11</v>
       </c>
@@ -2028,14 +2177,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967295" orientation="portrait" r:id="rId1" verticalDpi="4294967295"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
@@ -2043,13 +2192,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="35.5703125" collapsed="true"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="35.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2119,25 +2268,25 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967295" orientation="portrait" r:id="rId1" verticalDpi="4294967295"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2154,10 +2303,10 @@
         <v>192</v>
       </c>
       <c r="E1" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="F1" s="14" t="s">
         <v>197</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2168,27 +2317,25 @@
         <v>14</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>193</v>
       </c>
-      <c r="E2" s="17" t="s">
-        <v>201</v>
-      </c>
+      <c r="E2" s="17"/>
       <c r="F2" s="17" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967295" orientation="portrait" r:id="rId1" verticalDpi="4294967295"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
@@ -2196,20 +2343,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -2308,15 +2455,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -2324,11 +2471,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="63.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="63.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2379,15 +2526,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
@@ -2395,10 +2542,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2431,45 +2578,45 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:X2"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="38.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="30.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="38.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:23">
+    <row r="1" spans="1:23" s="1" customFormat="1">
       <c r="A1" s="26" t="s">
         <v>11</v>
       </c>
@@ -2627,16 +2774,110 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="46" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>201</v>
+      </c>
+      <c r="D1" s="43" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="43" t="s">
+        <v>148</v>
+      </c>
+      <c r="H1" s="41" t="s">
+        <v>203</v>
+      </c>
+      <c r="I1" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="J1" s="43" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="47" t="s">
+        <v>205</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>206</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>207</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>152</v>
+      </c>
+      <c r="F2" s="48" t="s">
+        <v>151</v>
+      </c>
+      <c r="G2" s="49" t="s">
+        <v>208</v>
+      </c>
+      <c r="H2" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="I2" s="42" t="s">
+        <v>209</v>
+      </c>
+      <c r="J2" s="45" t="s">
+        <v>210</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D2"/>
@@ -2644,10 +2885,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2679,14 +2920,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967295" orientation="portrait" r:id="rId1" verticalDpi="4294967295"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N1" sqref="N1:N2"/>
@@ -2694,19 +2935,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="5" max="7" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="7" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" ht="15.75" r="1" s="1" spans="1:13" thickBot="1">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -2747,7 +2988,7 @@
         <v>85</v>
       </c>
     </row>
-    <row ht="60.75" r="2" spans="1:13" thickBot="1">
+    <row r="2" spans="1:13" ht="60.75" thickBot="1">
       <c r="A2" s="13" t="s">
         <v>13</v>
       </c>
@@ -2790,16 +3031,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -2807,9 +3048,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2836,118 +3077,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
-    <col min="5" max="6" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:10">
-      <c r="A1" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="G1" s="36" t="s">
-        <v>128</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="G2" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="H3" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="H4" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
-  </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967295" orientation="portrait" r:id="rId2" verticalDpi="4294967295"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Hospital renewal and Add multiple risk test code
</commit_message>
<xml_diff>
--- a/src/main/resources/Form_Data.xlsx
+++ b/src/main/resources/Form_Data.xlsx
@@ -4,40 +4,41 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2448" windowWidth="20580" windowHeight="11076" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="2448" windowWidth="20580" windowHeight="11076"/>
   </bookViews>
   <sheets>
-    <sheet name="TC42252" sheetId="27" r:id="rId1"/>
-    <sheet name="TC42155" sheetId="26" r:id="rId2"/>
-    <sheet name="TC42203" sheetId="25" r:id="rId3"/>
-    <sheet name="TC43768" sheetId="24" r:id="rId4"/>
-    <sheet name="TC42246" sheetId="23" r:id="rId5"/>
-    <sheet name="TC42403" sheetId="28" r:id="rId6"/>
-    <sheet name="TC42249" sheetId="22" r:id="rId7"/>
-    <sheet name="TC42400" sheetId="12" r:id="rId8"/>
-    <sheet name="TC43666" sheetId="14" r:id="rId9"/>
-    <sheet name="TC42243" sheetId="16" r:id="rId10"/>
-    <sheet name="TC42405" sheetId="15" r:id="rId11"/>
-    <sheet name="TC42665" sheetId="2" r:id="rId12"/>
-    <sheet name="TC42399" sheetId="20" r:id="rId13"/>
-    <sheet name="TC42404" sheetId="1" r:id="rId14"/>
-    <sheet name="TC42239" sheetId="3" r:id="rId15"/>
-    <sheet name="TC42242" sheetId="4" r:id="rId16"/>
-    <sheet name="TC42238" sheetId="5" r:id="rId17"/>
-    <sheet name="TC42245" sheetId="6" r:id="rId18"/>
-    <sheet name="TC42530" sheetId="8" r:id="rId19"/>
-    <sheet name="TC42536" sheetId="9" r:id="rId20"/>
-    <sheet name="TC42253" sheetId="10" r:id="rId21"/>
-    <sheet name="TC42240" sheetId="17" r:id="rId22"/>
-    <sheet name="TC42247" sheetId="18" r:id="rId23"/>
-    <sheet name="TC42250" sheetId="19" r:id="rId24"/>
+    <sheet name="TC42244" sheetId="29" r:id="rId1"/>
+    <sheet name="TC42252" sheetId="27" r:id="rId2"/>
+    <sheet name="TC42155" sheetId="26" r:id="rId3"/>
+    <sheet name="TC42203" sheetId="25" r:id="rId4"/>
+    <sheet name="TC43768" sheetId="24" r:id="rId5"/>
+    <sheet name="TC42246" sheetId="23" r:id="rId6"/>
+    <sheet name="TC42403" sheetId="28" r:id="rId7"/>
+    <sheet name="TC42249" sheetId="22" r:id="rId8"/>
+    <sheet name="TC42400" sheetId="12" r:id="rId9"/>
+    <sheet name="TC43666" sheetId="14" r:id="rId10"/>
+    <sheet name="TC42243" sheetId="16" r:id="rId11"/>
+    <sheet name="TC42405" sheetId="15" r:id="rId12"/>
+    <sheet name="TC42665" sheetId="2" r:id="rId13"/>
+    <sheet name="TC42399" sheetId="20" r:id="rId14"/>
+    <sheet name="TC42404" sheetId="1" r:id="rId15"/>
+    <sheet name="TC42239" sheetId="3" r:id="rId16"/>
+    <sheet name="TC42242" sheetId="4" r:id="rId17"/>
+    <sheet name="TC42238" sheetId="5" r:id="rId18"/>
+    <sheet name="TC42245" sheetId="6" r:id="rId19"/>
+    <sheet name="TC42530" sheetId="8" r:id="rId20"/>
+    <sheet name="TC42536" sheetId="9" r:id="rId21"/>
+    <sheet name="TC42253" sheetId="10" r:id="rId22"/>
+    <sheet name="TC42240" sheetId="17" r:id="rId23"/>
+    <sheet name="TC42247" sheetId="18" r:id="rId24"/>
+    <sheet name="TC42250" sheetId="19" r:id="rId25"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="348">
   <si>
     <t>City</t>
   </si>
@@ -513,9 +514,6 @@
     <t>Renewal</t>
   </si>
   <si>
-    <t>Renewal Quote</t>
-  </si>
-  <si>
     <t>optionValue</t>
   </si>
   <si>
@@ -858,9 +856,6 @@
     <t>policyActionValue</t>
   </si>
   <si>
-    <t>saveAsPolicyValueRenewal</t>
-  </si>
-  <si>
     <t>vendorIDValue</t>
   </si>
   <si>
@@ -1042,6 +1037,51 @@
   </si>
   <si>
     <t>Lockton Companies (CO) (25, Med. Mal. PL, 01/01/1901 - 01/01/3000)</t>
+  </si>
+  <si>
+    <t>Quarterly</t>
+  </si>
+  <si>
+    <t>billingFrequency</t>
+  </si>
+  <si>
+    <t>screenShotName</t>
+  </si>
+  <si>
+    <t>ChangeBillingParameters</t>
+  </si>
+  <si>
+    <t>01/01/2014</t>
+  </si>
+  <si>
+    <t>Underwriter</t>
+  </si>
+  <si>
+    <t>teamNameType</t>
+  </si>
+  <si>
+    <t>3505510</t>
+  </si>
+  <si>
+    <t>quoteDescriptionText</t>
+  </si>
+  <si>
+    <t>09100510</t>
+  </si>
+  <si>
+    <t>saveAsPolicyDDLValue</t>
+  </si>
+  <si>
+    <t>RENQUOTE</t>
+  </si>
+  <si>
+    <t>policyPhaseValue</t>
+  </si>
+  <si>
+    <t>riskTypeValue</t>
+  </si>
+  <si>
+    <t>Phy Surg</t>
   </si>
 </sst>
 </file>
@@ -1295,7 +1335,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1372,9 +1412,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1424,6 +1461,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1729,127 +1769,196 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="15" thickBot="1">
       <c r="A1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="55" t="s">
-        <v>153</v>
-      </c>
-      <c r="D1" s="35" t="s">
-        <v>197</v>
-      </c>
-      <c r="E1" s="35" t="s">
-        <v>295</v>
-      </c>
-      <c r="F1" s="35" t="s">
-        <v>296</v>
-      </c>
-      <c r="G1" s="35" t="s">
-        <v>297</v>
-      </c>
-      <c r="H1" s="35" t="s">
-        <v>274</v>
-      </c>
-      <c r="I1" s="35" t="s">
-        <v>298</v>
-      </c>
-      <c r="J1" s="35" t="s">
-        <v>299</v>
-      </c>
-      <c r="K1" s="35" t="s">
-        <v>300</v>
-      </c>
-      <c r="L1" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" s="33" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="15" thickBot="1">
+      <c r="C1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" thickBot="1">
       <c r="A2" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="B2" s="43" t="s">
-        <v>188</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>316</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>302</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>303</v>
-      </c>
-      <c r="F2" s="37" t="s">
-        <v>304</v>
-      </c>
-      <c r="G2" s="37" t="s">
-        <v>305</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>306</v>
-      </c>
-      <c r="I2" s="37" t="s">
-        <v>307</v>
+      <c r="C2" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="D2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="21.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="24.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="19.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="19.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>95</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>308</v>
-      </c>
-      <c r="K2" s="37" t="s">
-        <v>309</v>
-      </c>
-      <c r="L2" s="27"/>
-      <c r="M2" s="56" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="15.6" customHeight="1">
-      <c r="F3" s="37" t="s">
-        <v>311</v>
-      </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="10" t="s">
-        <v>312</v>
-      </c>
-      <c r="I3" s="57" t="s">
-        <v>313</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="58" t="s">
-        <v>315</v>
+        <v>94</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1860,7 +1969,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1894,10 +2003,10 @@
         <v>138</v>
       </c>
       <c r="F1" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="G1" s="31" t="s">
         <v>159</v>
-      </c>
-      <c r="G1" s="31" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1917,10 +2026,10 @@
         <v>155</v>
       </c>
       <c r="F2" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>161</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -1931,7 +2040,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1983,7 +2092,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X4"/>
   <sheetViews>
@@ -2180,7 +2289,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -2204,14 +2313,14 @@
       <c r="A1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="41" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" s="35" t="s">
         <v>183</v>
-      </c>
-      <c r="D1" s="35" t="s">
-        <v>184</v>
       </c>
       <c r="E1" s="35" t="s">
         <v>139</v>
@@ -2223,10 +2332,10 @@
         <v>138</v>
       </c>
       <c r="H1" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="I1" s="33" t="s">
         <v>185</v>
-      </c>
-      <c r="I1" s="33" t="s">
-        <v>186</v>
       </c>
       <c r="J1" s="35" t="s">
         <v>140</v>
@@ -2234,34 +2343,34 @@
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1">
       <c r="A2" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="42" t="s">
         <v>187</v>
-      </c>
-      <c r="B2" s="43" t="s">
-        <v>188</v>
       </c>
       <c r="C2" s="37" t="s">
         <v>24</v>
       </c>
       <c r="D2" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="G2" s="40" t="s">
         <v>189</v>
-      </c>
-      <c r="E2" s="40" t="s">
-        <v>142</v>
-      </c>
-      <c r="F2" s="40" t="s">
-        <v>141</v>
-      </c>
-      <c r="G2" s="41" t="s">
-        <v>190</v>
       </c>
       <c r="H2" s="34" t="s">
         <v>133</v>
       </c>
       <c r="I2" s="34" t="s">
+        <v>190</v>
+      </c>
+      <c r="J2" s="37" t="s">
         <v>191</v>
-      </c>
-      <c r="J2" s="37" t="s">
-        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -2272,7 +2381,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -2297,29 +2406,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="49" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>250</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>251</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>253</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>254</v>
       </c>
       <c r="I1" s="35" t="s">
         <v>9</v>
@@ -2328,48 +2437,48 @@
         <v>10</v>
       </c>
       <c r="K1" s="35" t="s">
+        <v>254</v>
+      </c>
+      <c r="L1" s="35" t="s">
         <v>255</v>
-      </c>
-      <c r="L1" s="35" t="s">
-        <v>256</v>
       </c>
       <c r="M1" s="35" t="s">
         <v>75</v>
       </c>
       <c r="N1" s="35" t="s">
+        <v>256</v>
+      </c>
+      <c r="O1" s="35" t="s">
         <v>257</v>
       </c>
-      <c r="O1" s="35" t="s">
+    </row>
+    <row r="2" spans="1:15" ht="43.2">
+      <c r="A2" s="38" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" s="50" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="43.2">
-      <c r="A2" s="39" t="s">
-        <v>187</v>
-      </c>
-      <c r="B2" s="36" t="s">
-        <v>188</v>
-      </c>
-      <c r="C2" s="51" t="s">
+      <c r="D2" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="38">
+        <v>471</v>
+      </c>
+      <c r="H2" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>259</v>
-      </c>
-      <c r="D2" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="39">
-        <v>471</v>
-      </c>
-      <c r="H2" s="52" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>260</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>12</v>
@@ -2383,11 +2492,11 @@
       <c r="M2" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="N2" s="53" t="s">
+      <c r="N2" s="52" t="s">
+        <v>260</v>
+      </c>
+      <c r="O2" s="37" t="s">
         <v>261</v>
-      </c>
-      <c r="O2" s="37" t="s">
-        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -2399,12 +2508,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCellId="1" sqref="A2:XFD2 A1:XFD1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2418,22 +2527,22 @@
       <c r="A1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="41" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>138</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" thickBot="1">
       <c r="A2" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="B2" s="43" t="s">
-        <v>188</v>
-      </c>
       <c r="C2" s="10" t="s">
-        <v>194</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -2445,7 +2554,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
@@ -2555,7 +2664,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
@@ -2610,7 +2719,7 @@
         <v>138</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1">
@@ -2642,7 +2751,7 @@
         <v>134</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="K2" s="22" t="s">
         <v>133</v>
@@ -2686,7 +2795,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -2727,7 +2836,7 @@
         <v>125</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>138</v>
@@ -2745,57 +2854,57 @@
         <v>115</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>79</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>82</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15" thickBot="1">
       <c r="A2" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="42" t="s">
         <v>187</v>
-      </c>
-      <c r="B2" s="43" t="s">
-        <v>188</v>
       </c>
       <c r="C2" t="s">
         <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E2" t="s">
         <v>39</v>
       </c>
       <c r="F2" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="G2" t="s">
         <v>267</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" s="15" t="s">
         <v>268</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>269</v>
       </c>
       <c r="I2" t="s">
         <v>130</v>
       </c>
       <c r="J2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K2" t="s">
         <v>120</v>
       </c>
       <c r="L2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="M2" t="s">
         <v>133</v>
@@ -2812,7 +2921,140 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="15" thickBot="1">
+      <c r="A1" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>293</v>
+      </c>
+      <c r="F1" s="35" t="s">
+        <v>294</v>
+      </c>
+      <c r="G1" s="35" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="I1" s="35" t="s">
+        <v>296</v>
+      </c>
+      <c r="J1" s="35" t="s">
+        <v>297</v>
+      </c>
+      <c r="K1" s="35" t="s">
+        <v>298</v>
+      </c>
+      <c r="L1" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="33" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15" thickBot="1">
+      <c r="A2" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>300</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>302</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>303</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>305</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="K2" s="37" t="s">
+        <v>307</v>
+      </c>
+      <c r="L2" s="27"/>
+      <c r="M2" s="55" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.6" customHeight="1">
+      <c r="F3" s="37" t="s">
+        <v>309</v>
+      </c>
+      <c r="G3" s="37"/>
+      <c r="H3" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="I3" s="56" t="s">
+        <v>311</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="57" t="s">
+        <v>313</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -2830,52 +3072,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1">
-      <c r="A1" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="35" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1">
-      <c r="A2" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="B2" s="43" t="s">
-        <v>188</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>194</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2920,7 +3117,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
@@ -2946,241 +3143,241 @@
       <c r="A1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="41" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" s="46" customFormat="1" ht="15" thickBot="1">
-      <c r="A2" s="44" t="s">
+    <row r="2" spans="1:12" s="45" customFormat="1" ht="15" thickBot="1">
+      <c r="A2" s="43" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="44" t="s">
         <v>187</v>
       </c>
-      <c r="B2" s="45" t="s">
-        <v>188</v>
-      </c>
-      <c r="C2" s="46" t="s">
-        <v>332</v>
-      </c>
-      <c r="D2" s="46" t="s">
-        <v>331</v>
-      </c>
-      <c r="E2" s="46" t="s">
-        <v>302</v>
-      </c>
-      <c r="F2" s="47" t="s">
-        <v>303</v>
-      </c>
-      <c r="G2" s="47" t="s">
+      <c r="C2" s="45" t="s">
+        <v>330</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>329</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>300</v>
+      </c>
+      <c r="F2" s="46" t="s">
+        <v>301</v>
+      </c>
+      <c r="G2" s="46" t="s">
+        <v>202</v>
+      </c>
+      <c r="H2" s="46" t="s">
         <v>203</v>
       </c>
-      <c r="H2" s="47" t="s">
+      <c r="I2" s="45" t="s">
         <v>204</v>
       </c>
-      <c r="I2" s="46" t="s">
+      <c r="J2" s="45" t="s">
         <v>205</v>
-      </c>
-      <c r="J2" s="46" t="s">
-        <v>206</v>
       </c>
       <c r="K2"/>
     </row>
     <row r="3" spans="1:12">
       <c r="G3" t="s">
+        <v>206</v>
+      </c>
+      <c r="H3" t="s">
         <v>207</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" s="45" t="s">
         <v>208</v>
       </c>
-      <c r="I3" s="46" t="s">
+      <c r="J3" s="45" t="s">
         <v>209</v>
-      </c>
-      <c r="J3" s="46" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="G4" t="s">
+        <v>210</v>
+      </c>
+      <c r="H4" t="s">
         <v>211</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>212</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>213</v>
-      </c>
-      <c r="J4" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="G5" t="s">
+        <v>214</v>
+      </c>
+      <c r="H5" t="s">
         <v>215</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>216</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>217</v>
-      </c>
-      <c r="J5" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="G6" t="s">
+        <v>218</v>
+      </c>
+      <c r="H6" t="s">
         <v>219</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>220</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>221</v>
-      </c>
-      <c r="J6" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="G7" t="s">
+        <v>222</v>
+      </c>
+      <c r="H7" t="s">
         <v>223</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>224</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>225</v>
-      </c>
-      <c r="J7" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="I8" t="s">
+        <v>226</v>
+      </c>
+      <c r="J8" s="45" t="s">
         <v>227</v>
-      </c>
-      <c r="J8" s="46" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="I9" t="s">
+        <v>228</v>
+      </c>
+      <c r="J9" s="45" t="s">
         <v>229</v>
-      </c>
-      <c r="J9" s="46" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="I10" t="s">
+        <v>230</v>
+      </c>
+      <c r="J10" s="45" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="I11" s="45" t="s">
         <v>231</v>
       </c>
-      <c r="J10" s="46" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="I11" s="46" t="s">
+      <c r="J11" s="45" t="s">
         <v>232</v>
       </c>
-      <c r="J11" s="46" t="s">
+    </row>
+    <row r="12" spans="1:12">
+      <c r="I12" s="45" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="I12" s="46" t="s">
+      <c r="J12" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="J12" s="46" t="s">
+    </row>
+    <row r="13" spans="1:12">
+      <c r="I13" s="45" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="I13" s="46" t="s">
+      <c r="J13" s="45" t="s">
         <v>236</v>
       </c>
-      <c r="J13" s="46" t="s">
+    </row>
+    <row r="14" spans="1:12">
+      <c r="I14" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" s="45" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
-      <c r="I14" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="J14" s="46" t="s">
+    <row r="15" spans="1:12">
+      <c r="I15" s="45" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="I15" s="46" t="s">
+      <c r="J15" s="45" t="s">
         <v>239</v>
       </c>
-      <c r="J15" s="46" t="s">
+    </row>
+    <row r="16" spans="1:12">
+      <c r="I16" s="45" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="I16" s="46" t="s">
+      <c r="J16" s="45" t="s">
         <v>241</v>
       </c>
-      <c r="J16" s="46" t="s">
+    </row>
+    <row r="17" spans="9:10">
+      <c r="I17" s="45" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="17" spans="9:10">
-      <c r="I17" s="46" t="s">
+      <c r="J17" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="J17" s="46" t="s">
+    </row>
+    <row r="18" spans="9:10">
+      <c r="I18" s="45" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="18" spans="9:10">
-      <c r="I18" s="46" t="s">
+      <c r="J18" s="45" t="s">
         <v>245</v>
       </c>
-      <c r="J18" s="46" t="s">
+    </row>
+    <row r="19" spans="9:10">
+      <c r="I19" s="45" t="s">
+        <v>223</v>
+      </c>
+      <c r="J19" s="45" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="19" spans="9:10">
-      <c r="I19" s="46" t="s">
-        <v>224</v>
-      </c>
-      <c r="J19" s="46" t="s">
+    <row r="20" spans="9:10">
+      <c r="I20" s="45" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="20" spans="9:10">
-      <c r="I20" s="46" t="s">
+      <c r="J20" s="45" t="s">
         <v>248</v>
-      </c>
-      <c r="J20" s="46" t="s">
-        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -3191,7 +3388,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
@@ -3241,7 +3438,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>141</v>
@@ -3302,7 +3499,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
@@ -3332,7 +3529,7 @@
         <v>138</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E1" s="24" t="s">
         <v>58</v>
@@ -3352,39 +3549,39 @@
         <v>8</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>24</v>
       </c>
       <c r="F2" s="26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G2" s="27" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="G3" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="G4" s="32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="G5" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="G6" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -3393,7 +3590,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -3417,16 +3614,16 @@
         <v>6</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>175</v>
-      </c>
       <c r="E1" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>179</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -3437,14 +3634,14 @@
         <v>8</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -3454,6 +3651,51 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" thickBot="1">
+      <c r="A1" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickBot="1">
+      <c r="A2" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>193</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -3476,29 +3718,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="49" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>250</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>251</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>253</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>254</v>
       </c>
       <c r="I1" s="35" t="s">
         <v>9</v>
@@ -3507,48 +3749,48 @@
         <v>10</v>
       </c>
       <c r="K1" s="35" t="s">
+        <v>254</v>
+      </c>
+      <c r="L1" s="35" t="s">
         <v>255</v>
-      </c>
-      <c r="L1" s="35" t="s">
-        <v>256</v>
       </c>
       <c r="M1" s="35" t="s">
         <v>75</v>
       </c>
       <c r="N1" s="35" t="s">
+        <v>256</v>
+      </c>
+      <c r="O1" s="35" t="s">
         <v>257</v>
       </c>
-      <c r="O1" s="35" t="s">
+    </row>
+    <row r="2" spans="1:15" ht="43.2">
+      <c r="A2" s="38" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" s="50" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="43.2">
-      <c r="A2" s="39" t="s">
-        <v>187</v>
-      </c>
-      <c r="B2" s="36" t="s">
-        <v>188</v>
-      </c>
-      <c r="C2" s="51" t="s">
+      <c r="D2" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="38">
+        <v>471</v>
+      </c>
+      <c r="H2" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>259</v>
-      </c>
-      <c r="D2" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="39">
-        <v>471</v>
-      </c>
-      <c r="H2" s="52" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>260</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>12</v>
@@ -3562,11 +3804,11 @@
       <c r="M2" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="N2" s="53" t="s">
+      <c r="N2" s="52" t="s">
+        <v>260</v>
+      </c>
+      <c r="O2" s="37" t="s">
         <v>261</v>
-      </c>
-      <c r="O2" s="37" t="s">
-        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -3577,7 +3819,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE7"/>
   <sheetViews>
@@ -3708,13 +3950,13 @@
     </row>
     <row r="2" spans="1:31" ht="14.4" customHeight="1" thickBot="1">
       <c r="A2" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>188</v>
-      </c>
       <c r="C2" s="37" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>23</v>
@@ -3764,13 +4006,13 @@
       <c r="S2" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="T2" s="54" t="s">
+      <c r="T2" s="53" t="s">
         <v>44</v>
       </c>
       <c r="U2" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="V2" s="54" t="s">
+      <c r="V2" s="53" t="s">
         <v>48</v>
       </c>
       <c r="W2" s="37" t="s">
@@ -3798,12 +4040,12 @@
         <v>73</v>
       </c>
       <c r="AE2" s="37" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:31">
       <c r="C3" s="37" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G3" s="37" t="s">
         <v>13</v>
@@ -3894,12 +4136,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y3"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3939,49 +4181,49 @@
         <v>6</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>290</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>59</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>139</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>43</v>
@@ -3990,57 +4232,57 @@
         <v>51</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>60</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>321</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="15" thickBot="1">
       <c r="A2" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>188</v>
-      </c>
       <c r="C2" s="15" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="I2" s="15">
         <v>2</v>
       </c>
       <c r="J2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="K2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="L2" t="s">
         <v>59</v>
@@ -4048,17 +4290,17 @@
       <c r="M2" s="15">
         <v>1</v>
       </c>
-      <c r="N2" s="60" t="s">
-        <v>328</v>
+      <c r="N2" s="59" t="s">
+        <v>326</v>
       </c>
       <c r="O2" t="s">
         <v>24</v>
       </c>
       <c r="P2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="Q2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="R2" t="s">
         <v>141</v>
@@ -4067,73 +4309,27 @@
         <v>52</v>
       </c>
       <c r="T2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="U2" s="15" t="s">
         <v>26</v>
       </c>
       <c r="V2" s="15" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="W2" t="s">
-        <v>133</v>
+        <v>103</v>
       </c>
       <c r="X2" t="s">
+        <v>320</v>
+      </c>
+      <c r="Y2" t="s">
         <v>322</v>
       </c>
-      <c r="Y2" t="s">
-        <v>324</v>
-      </c>
     </row>
     <row r="3" spans="1:25">
-      <c r="C3" s="59">
+      <c r="C3" s="58">
         <v>9100437</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1">
-      <c r="A1" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1">
-      <c r="A2" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="C2" t="s">
-        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -4147,10 +4343,70 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF7"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="15" thickBot="1">
+      <c r="A1" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" thickBot="1">
+      <c r="A2" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D2" t="s">
+        <v>333</v>
+      </c>
+      <c r="E2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG7"/>
+  <sheetViews>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AG2" sqref="AG2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4162,7 +4418,7 @@
     <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1" collapsed="1"/>
@@ -4187,9 +4443,10 @@
     <col min="30" max="30" width="21.6640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="31" max="31" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="32" max="32" width="12.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="22.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="15" thickBot="1">
+    <row r="1" spans="1:33" ht="15" thickBot="1">
       <c r="A1" s="20" t="s">
         <v>5</v>
       </c>
@@ -4212,7 +4469,7 @@
         <v>61</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>62</v>
+        <v>339</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>63</v>
@@ -4280,22 +4537,25 @@
       <c r="AD1" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="61" t="s">
         <v>140</v>
       </c>
-      <c r="AF1" s="61" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" ht="14.4" customHeight="1" thickBot="1">
+      <c r="AF1" s="60" t="s">
+        <v>324</v>
+      </c>
+      <c r="AG1" s="60" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" ht="14.4" customHeight="1" thickBot="1">
       <c r="A2" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>188</v>
-      </c>
       <c r="C2" s="37" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>23</v>
@@ -4328,7 +4588,7 @@
         <v>29</v>
       </c>
       <c r="N2" s="15" t="s">
-        <v>25</v>
+        <v>337</v>
       </c>
       <c r="O2" t="s">
         <v>39</v>
@@ -4346,7 +4606,7 @@
         <v>50</v>
       </c>
       <c r="T2" s="16" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="U2" t="s">
         <v>49</v>
@@ -4379,13 +4639,16 @@
         <v>73</v>
       </c>
       <c r="AE2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AF2" s="15" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32">
+        <v>325</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33">
       <c r="G3" s="37" t="s">
         <v>13</v>
       </c>
@@ -4408,7 +4671,7 @@
         <v>30</v>
       </c>
       <c r="N3" s="15" t="s">
-        <v>25</v>
+        <v>337</v>
       </c>
       <c r="AA3" t="s">
         <v>34</v>
@@ -4423,7 +4686,16 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:32">
+    <row r="4" spans="1:33">
+      <c r="G4" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>338</v>
+      </c>
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
       <c r="J4" t="s">
         <v>28</v>
       </c>
@@ -4437,7 +4709,7 @@
         <v>31</v>
       </c>
       <c r="N4" s="15" t="s">
-        <v>25</v>
+        <v>337</v>
       </c>
       <c r="AA4" t="s">
         <v>28</v>
@@ -4446,92 +4718,25 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:32">
+    <row r="5" spans="1:33">
       <c r="M5" t="s">
         <v>32</v>
       </c>
       <c r="N5" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:32" ht="13.8" customHeight="1">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" ht="13.8" customHeight="1">
       <c r="M6" t="s">
         <v>33</v>
       </c>
       <c r="N6" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33">
       <c r="M7" t="s">
         <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="15" thickBot="1">
-      <c r="A1" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="35" t="s">
-        <v>272</v>
-      </c>
-      <c r="D1" s="35" t="s">
-        <v>273</v>
-      </c>
-      <c r="E1" s="35" t="s">
-        <v>265</v>
-      </c>
-      <c r="F1" s="35" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1">
-      <c r="A2" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="37" t="s">
-        <v>157</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>158</v>
-      </c>
-      <c r="E2" s="37" t="s">
-        <v>133</v>
-      </c>
-      <c r="F2" s="37" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -4544,122 +4749,81 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="21.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="24.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="19.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="18.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="19.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="28" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" thickBot="1">
+      <c r="A1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="N1" s="6" t="s">
+      <c r="C1" s="35" t="s">
+        <v>271</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>343</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>264</v>
+      </c>
+      <c r="F1" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>24</v>
+      <c r="I1" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickBot="1">
+      <c r="A2" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>344</v>
+      </c>
+      <c r="E2" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" s="62" t="s">
+        <v>157</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="I2" s="63" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>